<commit_message>
add attachments to test case
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Outlook Plugin\OutLookPlugin_auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624DFA3D-EB16-4582-8EEB-FE607C95940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3A10A9-2637-4B7F-8789-4661AEBABF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24390" yWindow="195" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23565" yWindow="1005" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,21 +59,7 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>Best Regards, 
-Nhut Dang 
-AS White Global 
-Australia | Vietnam 
-REE Tower, Level 7, 9 Doan Van Bo, Ward 9, Dictrict 4, HCMC, Vietnam 
-M: +84 77 663 0601</t>
-  </si>
-  <si>
     <t>Message footer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Begin body message:
-Claim number 00123456 realted to p.minh@aswhiteglobal.com. This claim is not paid yet. Please proceed
-</t>
   </si>
   <si>
     <t>Greetings: Dear MR/ MS Cappella</t>
@@ -135,6 +121,20 @@
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Begin body message:
+There is no claim found
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Regards, 
+Nhut Dang 
+AS White Global 
+Australia | Vietnam 
+REE Tower, Level 7, 9 Doan Van Bo, Ward 9, Dictrict 4, HCMC, Vietnam 
+</t>
   </si>
 </sst>
 </file>
@@ -505,15 +505,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -521,15 +521,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,26 +591,26 @@
     </row>
     <row r="5" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -660,15 +660,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -676,20 +676,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 4 basic test cases validate: red/green/yellow icons, and add 4 kinds of attachments
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Outlook Plugin\OutLookPlugin_auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3A10A9-2637-4B7F-8789-4661AEBABF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12B8A12-B607-42DC-9F36-F55EEE593A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23565" yWindow="1005" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23130" yWindow="1440" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="SheettestData" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>Receipient_SendTo</t>
   </si>
@@ -60,9 +62,6 @@
   </si>
   <si>
     <t>Message footer</t>
-  </si>
-  <si>
-    <t>Greetings: Dear MR/ MS Cappella</t>
   </si>
   <si>
     <t>BodyHeader</t>
@@ -134,6 +133,22 @@
 AS White Global 
 Australia | Vietnam 
 REE Tower, Level 7, 9 Doan Van Bo, Ward 9, Dictrict 4, HCMC, Vietnam 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test1@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12-3456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claimnumber 12-3456789. </t>
+  </si>
+  <si>
+    <t>test case 4 This test case will add 4 attachments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks
 </t>
   </si>
 </sst>
@@ -466,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,15 +520,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -521,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -529,7 +544,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ABB225-A725-4BD2-B0CF-E80ECCE5DFA1}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,9 +606,6 @@
     </row>
     <row r="5" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -602,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -610,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -624,11 +636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4742B8-E4D8-4791-98C5-C0A2A9018DFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D634E09-A0F0-41EC-8E50-F922078F17E8}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -660,15 +672,165 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D622FCFA-5597-4C30-BE61-D1643306D7D7}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="80.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4742B8-E4D8-4791-98C5-C0A2A9018DFA}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="80.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -676,7 +838,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -684,12 +846,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new commit for getting newest source for new laptop
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Outlook Plugin\OutLookPlugin_auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12B8A12-B607-42DC-9F36-F55EEE593A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2B7182-E379-46B5-A999-4AEDE3F3BAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23130" yWindow="1440" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="SheettestData" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Receipient_SendTo</t>
   </si>
@@ -46,19 +43,7 @@
     <t>BodyMess</t>
   </si>
   <si>
-    <t xml:space="preserve">A.DinhT@aswhiteglobal.com ;  T.Ngo@aswhiteglobal.com;  p.minh@aswhiteglobal.com  </t>
-  </si>
-  <si>
-    <t>t.xho@aswhiteglobal.com  ;  T.TranQ@aswhiteglobal.com  ;  cv.vo@aswhiteglobal.com  ;</t>
-  </si>
-  <si>
-    <t>test subject 2</t>
-  </si>
-  <si>
     <t>Red</t>
-  </si>
-  <si>
-    <t>Yellow</t>
   </si>
   <si>
     <t>Message footer</t>
@@ -107,49 +92,16 @@
     </r>
   </si>
   <si>
-    <t>tintin.heo@outlook.com</t>
-  </si>
-  <si>
     <t>test case 3</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Begin body message:
-You have Claim number 100045EML and 100068EML  matched with tintin.heo@outlook.com
-You will see claimnumber match with email =&gt; Icon will be green</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Begin body message:
-There is no claim found
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Regards, 
-Nhut Dang 
-AS White Global 
-Australia | Vietnam 
-REE Tower, Level 7, 9 Doan Van Bo, Ward 9, Dictrict 4, HCMC, Vietnam 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> test1@test.com</t>
   </si>
   <si>
     <t xml:space="preserve"> 12-3456789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Claimnumber 12-3456789. </t>
-  </si>
-  <si>
-    <t>test case 4 This test case will add 4 attachments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanks
-</t>
   </si>
 </sst>
 </file>
@@ -478,11 +430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D634E09-A0F0-41EC-8E50-F922078F17E8}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,25 +447,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -525,13 +471,13 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -541,15 +487,15 @@
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -559,88 +505,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ABB225-A725-4BD2-B0CF-E80ECCE5DFA1}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="54.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D634E09-A0F0-41EC-8E50-F922078F17E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A338582-4D7C-4A09-82BA-FCB1144D2E56}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -672,181 +541,36 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D622FCFA-5597-4C30-BE61-D1643306D7D7}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="80.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4742B8-E4D8-4791-98C5-C0A2A9018DFA}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="80.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>